<commit_message>
add automation for angular
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>Clone_Path</t>
   </si>
@@ -53,6 +53,12 @@
   </si>
   <si>
     <t>D:\\Backup\\FileName</t>
+  </si>
+  <si>
+    <t>D:\\Git\\demo\\petmatrix-backend-kku\\PetMatrix.API\\bin\\Release\\netcoreapp2.1\\publish</t>
+  </si>
+  <si>
+    <t>D:\Publish Files\PetMatrix\PetMatrixBackend</t>
   </si>
 </sst>
 </file>
@@ -385,7 +391,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -393,7 +399,7 @@
     <col min="1" max="1" width="75" customWidth="1"/>
     <col min="2" max="2" width="23.7109375" customWidth="1"/>
     <col min="3" max="3" width="89.5703125" customWidth="1"/>
-    <col min="4" max="4" width="35.28515625" customWidth="1"/>
+    <col min="4" max="4" width="47.140625" customWidth="1"/>
     <col min="5" max="5" width="24.28515625" customWidth="1"/>
     <col min="6" max="6" width="20.5703125" customWidth="1"/>
   </cols>
@@ -424,10 +430,10 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>

</xml_diff>